<commit_message>
use championship-specific categories for results
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionResults/6Attempts.xlsx
+++ b/owlcms/src/main/resources/templates/competitionResults/6Attempts.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3CDFBC-E130-4155-829C-F7CA344AA537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7397D29-C5A2-492C-8B41-0DF61B601D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$7:$U$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$7:$U$8</definedName>
     <definedName name="AFF.">Results!#REF!</definedName>
     <definedName name="Affiliation">Results!#REF!</definedName>
     <definedName name="Barre">#REF!</definedName>
@@ -25,7 +25,7 @@
     <definedName name="CategoryFilter">Results!#REF!</definedName>
     <definedName name="CLUB">Results!#REF!</definedName>
     <definedName name="Collet">#REF!</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="0">Results!$A$1:$CF$85</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="0">Results!$A$1:$CF$83</definedName>
     <definedName name="demandé">Results!#REF!</definedName>
     <definedName name="dernier">Results!#REF!</definedName>
     <definedName name="essais">Results!#REF!</definedName>
@@ -37,7 +37,7 @@
     <definedName name="InactiveGroupFilter">Results!#REF!</definedName>
     <definedName name="isSnatch">Results!#REF!</definedName>
     <definedName name="lbParKg">Results!#REF!</definedName>
-    <definedName name="LignesCalculs">Results!$11:$11</definedName>
+    <definedName name="LignesCalculs">Results!$9:$9</definedName>
     <definedName name="LignesEntête">Results!$1:$5</definedName>
     <definedName name="LignesOfficiels">Results!#REF!</definedName>
     <definedName name="M_F">Results!#REF!</definedName>
@@ -68,14 +68,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean-François Lamy</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9A4DBABE-1269-43CE-BADF-C534197E25AF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">jx:area(lastCell="V8")
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{D541F5E5-3FA4-4A5F-81A5-12431A6A680F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jx:each(items="lifters" var="l" lastCell="V8")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
-  <si>
-    <t>&lt;jx:forEach items="${lifters}" var="l" varStatus="lifterLoop"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/jx:forEach&gt;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>${l.lotNumber}</t>
   </si>
@@ -254,7 +285,7 @@
     <numFmt numFmtId="168" formatCode="0.000;;\-"/>
     <numFmt numFmtId="169" formatCode="0;\-;\-"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -379,6 +410,12 @@
       <sz val="10"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -870,6 +907,30 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -897,30 +958,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1381,11 +1418,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X111"/>
+  <dimension ref="A1:X109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -1417,7 +1454,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="33"/>
@@ -1426,10 +1463,10 @@
       <c r="F1" s="33"/>
       <c r="G1" s="14"/>
       <c r="J1" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L1" s="35"/>
       <c r="M1" s="36"/>
@@ -1445,15 +1482,15 @@
     </row>
     <row r="2" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="5"/>
       <c r="J2" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L2" s="42"/>
       <c r="M2" s="43"/>
@@ -1462,36 +1499,36 @@
       <c r="P2" s="45"/>
       <c r="Q2" s="46"/>
       <c r="R2" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="S2" s="47" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T2" s="48"/>
       <c r="U2" s="48"/>
     </row>
     <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="50"/>
       <c r="J3" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="72" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
+        <v>32</v>
+      </c>
+      <c r="K3" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="51"/>
       <c r="R3" s="23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S3" s="52" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T3" s="53"/>
       <c r="U3" s="53"/>
@@ -1499,17 +1536,17 @@
     </row>
     <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="32"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="J4" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L4"/>
       <c r="M4" s="3"/>
@@ -1526,64 +1563,64 @@
       <c r="H6" s="8"/>
       <c r="I6" s="10"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="68"/>
-      <c r="M6" s="69"/>
+      <c r="K6" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="60"/>
+      <c r="M6" s="61"/>
       <c r="N6" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="61"/>
+      <c r="R6" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="O6" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="S6" s="65" t="s">
+      <c r="T6" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="T6" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="U6" s="59" t="s">
+      <c r="V6" s="67" t="s">
         <v>53</v>
-      </c>
-      <c r="V6" s="61" t="s">
-        <v>55</v>
       </c>
       <c r="X6"/>
     </row>
     <row r="7" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>48</v>
-      </c>
       <c r="D7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="H7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="69"/>
-      <c r="G7" s="12" t="s">
+      <c r="I7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="K7" s="11">
         <v>1</v>
@@ -1595,7 +1632,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O7" s="11">
         <v>1</v>
@@ -1607,133 +1644,98 @@
         <v>3</v>
       </c>
       <c r="R7" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="72"/>
+      <c r="T7" s="70"/>
+      <c r="U7" s="66"/>
+      <c r="V7" s="68"/>
+    </row>
+    <row r="8" spans="1:24" s="20" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="63"/>
+      <c r="G8" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="R8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="S8" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="S7" s="66"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="62"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-    </row>
-    <row r="9" spans="1:24" s="20" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="71"/>
-      <c r="G9" s="57" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="58" t="s">
+      <c r="U8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="P9" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="R9" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="S9" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="T9" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="U9" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="V9" s="22" t="s">
-        <v>30</v>
-      </c>
+      <c r="V8" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="M9"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="1"/>
+      <c r="R9"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="13"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
+      <c r="F10" s="1"/>
+      <c r="U10" s="13"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="1"/>
-      <c r="M11"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="1"/>
-      <c r="R11"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F12" s="1"/>
@@ -1748,6 +1750,8 @@
       <c r="U14" s="13"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="1"/>
       <c r="U15" s="13"/>
     </row>
@@ -1755,57 +1759,53 @@
       <c r="F16" s="1"/>
       <c r="U16" s="13"/>
     </row>
-    <row r="17" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+    <row r="17" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F17" s="1"/>
       <c r="U17" s="13"/>
     </row>
-    <row r="18" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F18" s="1"/>
-      <c r="U18" s="13"/>
-    </row>
-    <row r="19" spans="4:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F19" s="1"/>
-      <c r="U19" s="13"/>
-    </row>
-    <row r="20" spans="4:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.2">
@@ -2038,38 +2038,28 @@
     </row>
     <row r="109" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F109" s="1"/>
-    </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F110" s="1"/>
-    </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F111" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="9">
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K3:O3"/>
     <mergeCell ref="U6:U7"/>
     <mergeCell ref="V6:V7"/>
     <mergeCell ref="T6:T7"/>
     <mergeCell ref="S6:S7"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="K3:O3"/>
   </mergeCells>
-  <conditionalFormatting sqref="D9:E9 D10:F10">
+  <conditionalFormatting sqref="D8:E8">
     <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation showErrorMessage="1" sqref="K4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="H9" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="H10" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>0</formula1>
-      <formula2>200</formula2>
-    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="H8" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="www.federation.org" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2078,5 +2068,6 @@
   <pageMargins left="0.31496062992125984" right="0.35433070866141736" top="0.39370078740157483" bottom="0.47244094488188981" header="0.51181102362204722" footer="0.23622047244094491"/>
   <pageSetup paperSize="5" scale="85" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove custom USAW document logic
Results: Move conditional group label logic into templates
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionResults/6Attempts.xlsx
+++ b/owlcms/src/main/resources/templates/competitionResults/6Attempts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgonzalez/Projects/Misc/owlcms4/owlcms/src/main/resources/templates/competitionResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7397D29-C5A2-492C-8B41-0DF61B601D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E062994-CA3C-AC48-876D-F0BC0AAB1D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="2300" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>${l.lotNumber}</t>
   </si>
@@ -171,9 +171,6 @@
     <t>${competition.competitionOrganizer}</t>
   </si>
   <si>
-    <t>${session.name}</t>
-  </si>
-  <si>
     <t>${competition.federation}</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
   </si>
   <si>
     <t xml:space="preserve">${t.get("Competition.competitionOrganizer")} : </t>
-  </si>
-  <si>
-    <t>${t.get("Group")} :</t>
   </si>
   <si>
     <t>${t.get("LastName")}</t>
@@ -907,6 +901,34 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -930,34 +952,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1424,37 +1418,35 @@
   </sheetPr>
   <dimension ref="A1:X109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
-    <col min="11" max="13" width="7.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="3" customWidth="1"/>
-    <col min="16" max="18" width="7.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" customWidth="1"/>
-    <col min="22" max="23" width="10.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="1" customWidth="1"/>
+    <col min="11" max="13" width="7.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="3" customWidth="1"/>
+    <col min="16" max="18" width="7.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" customWidth="1"/>
+    <col min="20" max="20" width="8.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.1640625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="10.1640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="8.1640625" style="1" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="33"/>
@@ -1463,7 +1455,7 @@
       <c r="F1" s="33"/>
       <c r="G1" s="14"/>
       <c r="J1" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>17</v>
@@ -1482,15 +1474,15 @@
     </row>
     <row r="2" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="5"/>
       <c r="J2" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L2" s="42"/>
       <c r="M2" s="43"/>
@@ -1499,7 +1491,7 @@
       <c r="P2" s="45"/>
       <c r="Q2" s="46"/>
       <c r="R2" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S2" s="47" t="s">
         <v>19</v>
@@ -1507,25 +1499,25 @@
       <c r="T2" s="48"/>
       <c r="U2" s="48"/>
     </row>
-    <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="50"/>
       <c r="J3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="51"/>
       <c r="R3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S3" s="52" t="s">
         <v>20</v>
@@ -1534,20 +1526,16 @@
       <c r="U3" s="53"/>
       <c r="V3" s="54"/>
     </row>
-    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="32"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="J4" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="J4" s="23"/>
+      <c r="K4" s="9"/>
       <c r="L4"/>
       <c r="M4" s="3"/>
       <c r="N4" s="1"/>
@@ -1556,71 +1544,71 @@
       <c r="R4" s="23"/>
       <c r="S4" s="55"/>
     </row>
-    <row r="5" spans="1:24" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8"/>
       <c r="C6" s="9"/>
       <c r="H6" s="8"/>
       <c r="I6" s="10"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="68"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="V6" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="X6"/>
+    </row>
+    <row r="7" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="60"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="59" t="s">
+      <c r="B7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="61"/>
-      <c r="R6" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="S6" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="T6" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="U6" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="V6" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="X6"/>
-    </row>
-    <row r="7" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>46</v>
-      </c>
       <c r="D7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="69"/>
+      <c r="G7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="H7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="61"/>
-      <c r="G7" s="12" t="s">
+      <c r="I7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="K7" s="11">
         <v>1</v>
@@ -1632,7 +1620,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O7" s="11">
         <v>1</v>
@@ -1644,19 +1632,19 @@
         <v>3</v>
       </c>
       <c r="R7" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="S7" s="72"/>
-      <c r="T7" s="70"/>
-      <c r="U7" s="66"/>
-      <c r="V7" s="68"/>
-    </row>
-    <row r="8" spans="1:24" s="20" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="S7" s="66"/>
+      <c r="T7" s="64"/>
+      <c r="U7" s="60"/>
+      <c r="V7" s="62"/>
+    </row>
+    <row r="8" spans="1:24" s="20" customFormat="1" ht="21.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>0</v>
@@ -1664,10 +1652,10 @@
       <c r="D8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="63"/>
+      <c r="F8" s="71"/>
       <c r="G8" s="57" t="s">
         <v>4</v>
       </c>
@@ -1678,7 +1666,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="19" t="s">
         <v>10</v>
@@ -1708,16 +1696,16 @@
         <v>6</v>
       </c>
       <c r="T8" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U8" s="22" t="s">
         <v>7</v>
       </c>
       <c r="V8" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="H9" s="2"/>
@@ -1729,328 +1717,328 @@
       <c r="S9" s="1"/>
       <c r="T9" s="13"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
       <c r="F10" s="1"/>
       <c r="U10" s="13"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
       <c r="F11" s="1"/>
       <c r="U11" s="13"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
       <c r="F12" s="1"/>
       <c r="U12" s="13"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
       <c r="F13" s="1"/>
       <c r="U13" s="13"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
       <c r="F14" s="1"/>
       <c r="U14" s="13"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="1"/>
       <c r="U15" s="13"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
       <c r="F16" s="1"/>
       <c r="U16" s="13"/>
     </row>
-    <row r="17" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F17" s="1"/>
       <c r="U17" s="13"/>
     </row>
-    <row r="18" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="6:21" x14ac:dyDescent="0.15">
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F109" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="9">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="K3:O3"/>
     <mergeCell ref="U6:U7"/>
     <mergeCell ref="V6:V7"/>
     <mergeCell ref="T6:T7"/>
     <mergeCell ref="S6:S7"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="K3:O3"/>
   </mergeCells>
   <conditionalFormatting sqref="D8:E8">
     <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">

</xml_diff>